<commit_message>
added tables with foreign key to example excel
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
   <si>
     <t>Col1</t>
   </si>
@@ -251,6 +252,21 @@
   </si>
   <si>
     <t>11|12</t>
+  </si>
+  <si>
+    <t>Id [String]</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Id [String] {Tab2:Id}</t>
+  </si>
+  <si>
+    <t>a3</t>
   </si>
 </sst>
 </file>
@@ -390,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -412,6 +428,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -695,24 +715,24 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="11" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5703125" style="9" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="11" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
@@ -720,7 +740,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -750,7 +770,7 @@
       </c>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
@@ -782,7 +802,7 @@
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>42</v>
       </c>
@@ -814,7 +834,7 @@
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -828,7 +848,7 @@
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
@@ -840,7 +860,7 @@
       <c r="J6" s="15"/>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -852,7 +872,7 @@
       <c r="J7" s="10"/>
       <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -861,7 +881,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -893,7 +913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>5</v>
       </c>
@@ -926,7 +946,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>42</v>
       </c>
@@ -959,7 +979,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -972,7 +992,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
@@ -984,7 +1004,7 @@
       <c r="J13" s="10"/>
       <c r="K13" s="9"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -996,7 +1016,7 @@
       <c r="J14" s="10"/>
       <c r="K14" s="9"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
@@ -1010,7 +1030,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>17</v>
       </c>
@@ -1024,7 +1044,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>18</v>
       </c>
@@ -1038,12 +1058,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="5">
-        <v>43601.519112118054</v>
+        <v>43769.765087037034</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>14</v>
@@ -1052,7 +1072,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>34</v>
       </c>
@@ -1066,7 +1086,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>20</v>
       </c>
@@ -1074,17 +1094,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1101,7 +1121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>57</v>
       </c>
@@ -1123,7 +1143,7 @@
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>59</v>
       </c>
@@ -1145,7 +1165,7 @@
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1165,19 +1185,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>37</v>
       </c>
@@ -1191,7 +1211,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1205,7 +1225,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>69</v>
       </c>
@@ -1219,7 +1239,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>67</v>
       </c>
@@ -1233,7 +1253,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -1247,7 +1267,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>75</v>
       </c>
@@ -1261,7 +1281,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>73</v>
       </c>
@@ -1275,77 +1295,391 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
     </row>
-    <row r="17" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-    </row>
-    <row r="18" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-    </row>
-    <row r="19" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-    </row>
-    <row r="20" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-    </row>
-    <row r="21" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
+    <row r="17" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+    </row>
+    <row r="24" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+    </row>
+    <row r="29" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+    </row>
+    <row r="30" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+    </row>
+    <row r="31" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+    </row>
+    <row r="32" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+    </row>
+    <row r="33" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+    </row>
+    <row r="34" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+    </row>
+    <row r="35" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+    </row>
+    <row r="36" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+    </row>
+    <row r="37" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+    </row>
+    <row r="38" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+    </row>
+    <row r="39" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
+    </row>
+    <row r="40" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+    </row>
+    <row r="41" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+    </row>
+    <row r="42" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+    </row>
+    <row r="43" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+    </row>
+    <row r="44" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+    </row>
+    <row r="45" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+    </row>
+    <row r="46" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+    </row>
+    <row r="47" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
+    </row>
+    <row r="48" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+    </row>
+    <row r="49" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+    </row>
+    <row r="50" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+    </row>
+    <row r="51" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
+    </row>
+    <row r="52" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
+    </row>
+    <row r="53" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I53" s="12"/>
+      <c r="J53" s="12"/>
+      <c r="K53" s="12"/>
+    </row>
+    <row r="54" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
+      <c r="K54" s="12"/>
+    </row>
+    <row r="55" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
+    </row>
+    <row r="56" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12"/>
+    </row>
+    <row r="57" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
+    </row>
+    <row r="58" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+    </row>
+    <row r="59" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
+      <c r="K59" s="12"/>
+    </row>
+    <row r="60" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+    </row>
+    <row r="61" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="12"/>
+    </row>
+    <row r="62" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+    </row>
+    <row r="63" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="K63" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="6.28515625" style="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" style="22" collapsed="1"/>
+    <col min="4" max="4" width="11" style="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.140625" style="22" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="17">
+        <v>1</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>2</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="17">
+        <v>1</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="17">
+        <v>1</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="D6" s="17">
+        <v>2</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="D7" s="24">
+        <v>2</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>